<commit_message>
added relevant columns to template-backbone
</commit_message>
<xml_diff>
--- a/msAnalyzer/data/template-backbone.xlsx
+++ b/msAnalyzer/data/template-backbone.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gui/Git/labUtils/msAnalyzer/dataChol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gui/Git/labUtils/msAnalyzer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{06C08785-CF3A-9149-8B72-1F8BE5BB0674}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C62C6AFF-C8B6-C748-ABCF-E523A83929E7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="460" windowWidth="21100" windowHeight="14400" tabRatio="400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,6 @@
     <sheet name="STANDARD_NOT_LABELED" sheetId="7" r:id="rId2"/>
     <sheet name="STANDARD_LABELED" sheetId="4" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="135">
   <si>
     <t>A</t>
   </si>
@@ -429,6 +426,12 @@
   </si>
   <si>
     <t>30:5</t>
+  </si>
+  <si>
+    <t>VolumeOfDilution</t>
+  </si>
+  <si>
+    <t>VolumeOfSampleUsed</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1154,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1277,6 +1280,9 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -1406,863 +1412,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>neg</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>neg</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>S1</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>S2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>S3</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>S4</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>S5</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>S6</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Veh_09_N</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C9">
-            <v>72</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>GSK_10_N</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C10">
-            <v>54.599999999999909</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Veh_11_N</v>
-          </cell>
-          <cell r="B11" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C11">
-            <v>134.30000000000018</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>GSK_12_N</v>
-          </cell>
-          <cell r="B12" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C12">
-            <v>59.700000000000273</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Veh_13_N</v>
-          </cell>
-          <cell r="B13" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C13">
-            <v>65.099999999999909</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>GSK_14_N</v>
-          </cell>
-          <cell r="B14" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C14">
-            <v>88.700000000000273</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>Veh_15_N</v>
-          </cell>
-          <cell r="B15" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C15">
-            <v>117.30000000000018</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>GSK_16_N</v>
-          </cell>
-          <cell r="B16" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C16">
-            <v>80.5</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>Veh_25_N</v>
-          </cell>
-          <cell r="B17" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C17">
-            <v>50</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>GSK_26_N</v>
-          </cell>
-          <cell r="B18" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C18">
-            <v>74.5</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>Veh_27_N</v>
-          </cell>
-          <cell r="B19" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C19">
-            <v>78.800000000000182</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>GSK_28_N</v>
-          </cell>
-          <cell r="B20" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C20">
-            <v>50.400000000000091</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>Veh_29_N</v>
-          </cell>
-          <cell r="B21" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C21">
-            <v>101</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>GSK_30_N</v>
-          </cell>
-          <cell r="B22" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C22">
-            <v>106.29999999999973</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>Veh_31_N</v>
-          </cell>
-          <cell r="B23" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C23">
-            <v>96.5</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>GSK_32_N</v>
-          </cell>
-          <cell r="B24" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C24">
-            <v>69.200000000000273</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>Veh_01</v>
-          </cell>
-          <cell r="B25" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C25">
-            <v>72.900000000000091</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>GSK_02</v>
-          </cell>
-          <cell r="B26" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C26">
-            <v>47.300000000000182</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>Veh_03</v>
-          </cell>
-          <cell r="B27" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C27">
-            <v>52.400000000000091</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>GSK_04</v>
-          </cell>
-          <cell r="B28" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C28">
-            <v>79.099999999999909</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>Veh_05</v>
-          </cell>
-          <cell r="B29" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C29">
-            <v>52.599999999999909</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>GSK_06</v>
-          </cell>
-          <cell r="B30" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C30">
-            <v>70.800000000000182</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>Veh_07</v>
-          </cell>
-          <cell r="B31" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C31">
-            <v>65</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>GSK_08</v>
-          </cell>
-          <cell r="B32" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C32">
-            <v>73.5</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>Veh_17</v>
-          </cell>
-          <cell r="B33" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C33">
-            <v>49.200000000000273</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>GSK_18</v>
-          </cell>
-          <cell r="B34" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C34">
-            <v>57.699999999999818</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>Veh_19</v>
-          </cell>
-          <cell r="B35" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C35">
-            <v>72.300000000000182</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>GSK_20</v>
-          </cell>
-          <cell r="B36" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C36">
-            <v>64.300000000000182</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>Veh_21</v>
-          </cell>
-          <cell r="B37" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C37">
-            <v>50.299999999999727</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>GSK_22</v>
-          </cell>
-          <cell r="B38" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C38">
-            <v>53.5</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39" t="str">
-            <v>Veh_23</v>
-          </cell>
-          <cell r="B39" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C39">
-            <v>56.799999999999727</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40" t="str">
-            <v>GSK_24</v>
-          </cell>
-          <cell r="B40" t="str">
-            <v>ETV37</v>
-          </cell>
-          <cell r="C40">
-            <v>73.200000000000273</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41" t="str">
-            <v>Veh_1</v>
-          </cell>
-          <cell r="B41" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C41">
-            <v>40.100000000000364</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42" t="str">
-            <v>GSK_2</v>
-          </cell>
-          <cell r="B42" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C42">
-            <v>34.199999999999818</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43" t="str">
-            <v>Veh_3</v>
-          </cell>
-          <cell r="B43" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C43">
-            <v>28.400000000000091</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44" t="str">
-            <v>GSK_4</v>
-          </cell>
-          <cell r="B44" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C44">
-            <v>56.599999999999909</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45" t="str">
-            <v>Veh_5</v>
-          </cell>
-          <cell r="B45" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C45">
-            <v>55.800000000000182</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46" t="str">
-            <v>Veh_6</v>
-          </cell>
-          <cell r="B46" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C46">
-            <v>55.900000000000091</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47" t="str">
-            <v>GSK_7</v>
-          </cell>
-          <cell r="B47" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C47">
-            <v>31.699999999999818</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48" t="str">
-            <v>Veh_8</v>
-          </cell>
-          <cell r="B48" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C48">
-            <v>46.099999999999909</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49" t="str">
-            <v>GSK_9</v>
-          </cell>
-          <cell r="B49" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C49">
-            <v>52.099999999999909</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50" t="str">
-            <v>Veh_10</v>
-          </cell>
-          <cell r="B50" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C50">
-            <v>66.299999999999727</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51" t="str">
-            <v>GSK_11</v>
-          </cell>
-          <cell r="B51" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C51">
-            <v>59.700000000000273</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52" t="str">
-            <v>GSK_12</v>
-          </cell>
-          <cell r="B52" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C52">
-            <v>31.400000000000091</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53" t="str">
-            <v>GSK_13</v>
-          </cell>
-          <cell r="B53" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C53">
-            <v>69.099999999999909</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54" t="str">
-            <v>GSK_14</v>
-          </cell>
-          <cell r="B54" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C54">
-            <v>44.400000000000091</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55" t="str">
-            <v>Veh_15</v>
-          </cell>
-          <cell r="B55" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C55">
-            <v>68.5</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56" t="str">
-            <v>Veh_16</v>
-          </cell>
-          <cell r="B56" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C56">
-            <v>44.299999999999727</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57" t="str">
-            <v>Veh_17</v>
-          </cell>
-          <cell r="B57" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C57">
-            <v>43.199999999999818</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58" t="str">
-            <v>Veh_18</v>
-          </cell>
-          <cell r="B58" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C58">
-            <v>51.200000000000273</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59" t="str">
-            <v>GSK_19</v>
-          </cell>
-          <cell r="B59" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C59">
-            <v>56.599999999999909</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="A60" t="str">
-            <v>Veh_20</v>
-          </cell>
-          <cell r="B60" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C60">
-            <v>59.800000000000182</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="A61" t="str">
-            <v>GSK_21</v>
-          </cell>
-          <cell r="B61" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C61">
-            <v>72.900000000000091</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="A62" t="str">
-            <v>Veh_22</v>
-          </cell>
-          <cell r="B62" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C62">
-            <v>50.399999999999636</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="A63" t="str">
-            <v>GSK_23</v>
-          </cell>
-          <cell r="B63" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C63">
-            <v>52.099999999999909</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="A64" t="str">
-            <v>Veh_24</v>
-          </cell>
-          <cell r="B64" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C64">
-            <v>58.299999999999727</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="A65" t="str">
-            <v>GSK_25</v>
-          </cell>
-          <cell r="B65" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C65">
-            <v>53.199999999999818</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="A66" t="str">
-            <v>GSK_26</v>
-          </cell>
-          <cell r="B66" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C66">
-            <v>65.300000000000182</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="A67" t="str">
-            <v>Veh_27</v>
-          </cell>
-          <cell r="B67" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C67">
-            <v>43.300000000000182</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="A68" t="str">
-            <v>GSK_28</v>
-          </cell>
-          <cell r="B68" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C68">
-            <v>62.900000000000091</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="A69" t="str">
-            <v>Veh_29</v>
-          </cell>
-          <cell r="B69" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C69">
-            <v>62.199999999999818</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="A70" t="str">
-            <v>GSK_30</v>
-          </cell>
-          <cell r="B70" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C70">
-            <v>86.300000000000182</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="A71" t="str">
-            <v>Veh_31</v>
-          </cell>
-          <cell r="B71" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C71">
-            <v>63.5</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="A72" t="str">
-            <v>Veh_32</v>
-          </cell>
-          <cell r="B72" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C72">
-            <v>60.699999999999818</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="A73" t="str">
-            <v>GSK_33</v>
-          </cell>
-          <cell r="B73" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C73">
-            <v>53.900000000000091</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74" t="str">
-            <v>Veh_34</v>
-          </cell>
-          <cell r="B74" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C74">
-            <v>43.099999999999909</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="A75" t="str">
-            <v>GSK_35</v>
-          </cell>
-          <cell r="B75" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C75">
-            <v>70</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="A76" t="str">
-            <v>Veh_36</v>
-          </cell>
-          <cell r="B76" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C76">
-            <v>75.599999999999909</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="A77" t="str">
-            <v>GSK_37</v>
-          </cell>
-          <cell r="B77" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C77">
-            <v>64.699999999999818</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78" t="str">
-            <v>Veh_38</v>
-          </cell>
-          <cell r="B78" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C78">
-            <v>57.599999999999909</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79" t="str">
-            <v>GSK_39</v>
-          </cell>
-          <cell r="B79" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C79">
-            <v>77.699999999999818</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="A80" t="str">
-            <v>Veh_40</v>
-          </cell>
-          <cell r="B80" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C80">
-            <v>72.799999999999727</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="A81" t="str">
-            <v>GSK_41</v>
-          </cell>
-          <cell r="B81" t="str">
-            <v>ETV22</v>
-          </cell>
-          <cell r="C81">
-            <v>55.200000000000273</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2600,7 +1749,9 @@
     <col min="4" max="4" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="1000" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="1000" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" customHeight="1">
@@ -2621,6 +1772,12 @@
       </c>
       <c r="F1" s="53" t="s">
         <v>116</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="54" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15">

</xml_diff>

<commit_message>
added cholesterol in standard template
</commit_message>
<xml_diff>
--- a/msAnalyzer/data/template-backbone.xlsx
+++ b/msAnalyzer/data/template-backbone.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gui/Git/labUtils/msAnalyzer/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcalmettes/Git/labUtils/msAnalyzer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1E92D86F-275C-0448-982F-6F8D105C1711}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C55857BD-5CAA-B941-871B-73BF491ACBEA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="21100" windowHeight="14400" tabRatio="400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="21100" windowHeight="14400" tabRatio="400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAP" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="135">
   <si>
     <t>A</t>
   </si>
@@ -1256,18 +1256,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="25" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="25" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="45" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1280,6 +1268,30 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="25" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -1734,7 +1746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ALL101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -1752,427 +1764,427 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" customHeight="1">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="45" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15">
-      <c r="A2" s="50">
+      <c r="A2" s="42">
         <v>1</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="15">
-      <c r="A3" s="50">
+      <c r="A3" s="42">
         <v>1</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:8" ht="15">
-      <c r="A4" s="50">
+      <c r="A4" s="42">
         <v>1</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="51"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:8" ht="15">
-      <c r="A5" s="50">
+      <c r="A5" s="42">
         <v>1</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="43"/>
     </row>
     <row r="6" spans="1:8" ht="15">
-      <c r="A6" s="50">
+      <c r="A6" s="42">
         <v>1</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="51"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="43"/>
     </row>
     <row r="7" spans="1:8" ht="15">
-      <c r="A7" s="50">
+      <c r="A7" s="42">
         <v>1</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="51"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="1:8" ht="15">
-      <c r="A8" s="50">
+      <c r="A8" s="42">
         <v>1</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="43"/>
     </row>
     <row r="9" spans="1:8" ht="15">
-      <c r="A9" s="50">
+      <c r="A9" s="42">
         <v>1</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="51"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="43"/>
     </row>
     <row r="10" spans="1:8" ht="15">
-      <c r="A10" s="50">
+      <c r="A10" s="42">
         <v>2</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="51"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="15">
-      <c r="A11" s="50">
+      <c r="A11" s="42">
         <v>2</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="51"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="43"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="15">
-      <c r="A12" s="50">
+      <c r="A12" s="42">
         <v>2</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="43"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="15">
-      <c r="A13" s="50">
+      <c r="A13" s="42">
         <v>2</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="51"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="15">
-      <c r="A14" s="50">
+      <c r="A14" s="42">
         <v>2</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="51"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="15">
-      <c r="A15" s="50">
+      <c r="A15" s="42">
         <v>2</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="51"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="43"/>
     </row>
     <row r="16" spans="1:8" ht="15">
-      <c r="A16" s="50">
+      <c r="A16" s="42">
         <v>2</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="51"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:1000" ht="15">
-      <c r="A17" s="50">
+      <c r="A17" s="42">
         <v>2</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="51"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="43"/>
     </row>
     <row r="18" spans="1:1000" ht="15">
-      <c r="A18" s="50">
+      <c r="A18" s="42">
         <v>3</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="51"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="43"/>
     </row>
     <row r="19" spans="1:1000" ht="15">
-      <c r="A19" s="50">
+      <c r="A19" s="42">
         <v>3</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="51"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="43"/>
     </row>
     <row r="20" spans="1:1000" ht="15">
-      <c r="A20" s="50">
+      <c r="A20" s="42">
         <v>3</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="51"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="43"/>
     </row>
     <row r="21" spans="1:1000" ht="15">
-      <c r="A21" s="50">
+      <c r="A21" s="42">
         <v>3</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="51"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:1000" ht="15">
-      <c r="A22" s="50">
+      <c r="A22" s="42">
         <v>3</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="51"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:1000" ht="15">
-      <c r="A23" s="50">
+      <c r="A23" s="42">
         <v>3</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="51"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="43"/>
     </row>
     <row r="24" spans="1:1000" ht="15">
-      <c r="A24" s="50">
+      <c r="A24" s="42">
         <v>3</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="51"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
     </row>
     <row r="25" spans="1:1000" ht="15">
-      <c r="A25" s="50">
+      <c r="A25" s="42">
         <v>3</v>
       </c>
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="51"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="43"/>
     </row>
     <row r="26" spans="1:1000" ht="15">
-      <c r="A26" s="50">
+      <c r="A26" s="42">
         <v>4</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="51"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="43"/>
     </row>
     <row r="27" spans="1:1000" ht="15">
-      <c r="A27" s="50">
+      <c r="A27" s="42">
         <v>4</v>
       </c>
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="52" t="s">
+      <c r="C27" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="51"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="43"/>
     </row>
     <row r="28" spans="1:1000" ht="15">
-      <c r="A28" s="50">
+      <c r="A28" s="42">
         <v>4</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="52" t="s">
+      <c r="C28" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="51"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
     </row>
     <row r="29" spans="1:1000" ht="15">
-      <c r="A29" s="50">
+      <c r="A29" s="42">
         <v>4</v>
       </c>
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="52" t="s">
+      <c r="C29" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="51"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="43"/>
       <c r="ALE29"/>
       <c r="ALF29"/>
       <c r="ALG29"/>
@@ -2183,18 +2195,18 @@
       <c r="ALL29"/>
     </row>
     <row r="30" spans="1:1000" ht="15">
-      <c r="A30" s="50">
+      <c r="A30" s="42">
         <v>4</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="52" t="s">
+      <c r="C30" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="51"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="43"/>
       <c r="ALE30"/>
       <c r="ALF30"/>
       <c r="ALG30"/>
@@ -2205,18 +2217,18 @@
       <c r="ALL30"/>
     </row>
     <row r="31" spans="1:1000" ht="15">
-      <c r="A31" s="50">
+      <c r="A31" s="42">
         <v>4</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="52" t="s">
+      <c r="C31" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="51"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="43"/>
       <c r="ALE31"/>
       <c r="ALF31"/>
       <c r="ALG31"/>
@@ -2227,18 +2239,18 @@
       <c r="ALL31"/>
     </row>
     <row r="32" spans="1:1000" ht="15">
-      <c r="A32" s="50">
+      <c r="A32" s="42">
         <v>4</v>
       </c>
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="51"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="43"/>
       <c r="ALE32"/>
       <c r="ALF32"/>
       <c r="ALG32"/>
@@ -2249,18 +2261,18 @@
       <c r="ALL32"/>
     </row>
     <row r="33" spans="1:1000" ht="15">
-      <c r="A33" s="50">
+      <c r="A33" s="42">
         <v>4</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="C33" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="51"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="43"/>
       <c r="ALE33"/>
       <c r="ALF33"/>
       <c r="ALG33"/>
@@ -2271,18 +2283,18 @@
       <c r="ALL33"/>
     </row>
     <row r="34" spans="1:1000" ht="15">
-      <c r="A34" s="50">
+      <c r="A34" s="42">
         <v>5</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="52" t="s">
+      <c r="C34" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="51"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="43"/>
       <c r="ALE34"/>
       <c r="ALF34"/>
       <c r="ALG34"/>
@@ -2293,18 +2305,18 @@
       <c r="ALL34"/>
     </row>
     <row r="35" spans="1:1000" ht="15">
-      <c r="A35" s="50">
+      <c r="A35" s="42">
         <v>5</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="52" t="s">
+      <c r="C35" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="51"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="43"/>
       <c r="ALE35"/>
       <c r="ALF35"/>
       <c r="ALG35"/>
@@ -2315,18 +2327,18 @@
       <c r="ALL35"/>
     </row>
     <row r="36" spans="1:1000" ht="15">
-      <c r="A36" s="50">
+      <c r="A36" s="42">
         <v>5</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="51"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="43"/>
       <c r="ALE36"/>
       <c r="ALF36"/>
       <c r="ALG36"/>
@@ -2337,18 +2349,18 @@
       <c r="ALL36"/>
     </row>
     <row r="37" spans="1:1000" ht="15">
-      <c r="A37" s="50">
+      <c r="A37" s="42">
         <v>5</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="52" t="s">
+      <c r="C37" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="51"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="43"/>
       <c r="ALE37"/>
       <c r="ALF37"/>
       <c r="ALG37"/>
@@ -2359,18 +2371,18 @@
       <c r="ALL37"/>
     </row>
     <row r="38" spans="1:1000" ht="15">
-      <c r="A38" s="50">
+      <c r="A38" s="42">
         <v>5</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="52" t="s">
+      <c r="C38" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="51"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="43"/>
       <c r="ALE38"/>
       <c r="ALF38"/>
       <c r="ALG38"/>
@@ -2381,18 +2393,18 @@
       <c r="ALL38"/>
     </row>
     <row r="39" spans="1:1000" ht="15">
-      <c r="A39" s="50">
+      <c r="A39" s="42">
         <v>5</v>
       </c>
-      <c r="B39" s="50" t="s">
+      <c r="B39" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="52" t="s">
+      <c r="C39" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="51"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="43"/>
       <c r="ALE39"/>
       <c r="ALF39"/>
       <c r="ALG39"/>
@@ -2403,18 +2415,18 @@
       <c r="ALL39"/>
     </row>
     <row r="40" spans="1:1000" ht="15">
-      <c r="A40" s="50">
+      <c r="A40" s="42">
         <v>5</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="52" t="s">
+      <c r="C40" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="51"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="43"/>
       <c r="ALE40"/>
       <c r="ALF40"/>
       <c r="ALG40"/>
@@ -2425,18 +2437,18 @@
       <c r="ALL40"/>
     </row>
     <row r="41" spans="1:1000" ht="15">
-      <c r="A41" s="50">
+      <c r="A41" s="42">
         <v>5</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="51"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="43"/>
       <c r="ALE41"/>
       <c r="ALF41"/>
       <c r="ALG41"/>
@@ -2447,18 +2459,18 @@
       <c r="ALL41"/>
     </row>
     <row r="42" spans="1:1000" ht="15">
-      <c r="A42" s="50">
+      <c r="A42" s="42">
         <v>6</v>
       </c>
-      <c r="B42" s="50" t="s">
+      <c r="B42" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="52" t="s">
+      <c r="C42" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="51"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="43"/>
       <c r="ALE42"/>
       <c r="ALF42"/>
       <c r="ALG42"/>
@@ -2469,18 +2481,18 @@
       <c r="ALL42"/>
     </row>
     <row r="43" spans="1:1000" ht="15">
-      <c r="A43" s="50">
+      <c r="A43" s="42">
         <v>6</v>
       </c>
-      <c r="B43" s="50" t="s">
+      <c r="B43" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="52" t="s">
+      <c r="C43" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="51"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="43"/>
       <c r="ALE43"/>
       <c r="ALF43"/>
       <c r="ALG43"/>
@@ -2491,18 +2503,18 @@
       <c r="ALL43"/>
     </row>
     <row r="44" spans="1:1000" ht="15">
-      <c r="A44" s="50">
+      <c r="A44" s="42">
         <v>6</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="52" t="s">
+      <c r="C44" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="51"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="43"/>
       <c r="ALE44"/>
       <c r="ALF44"/>
       <c r="ALG44"/>
@@ -2513,18 +2525,18 @@
       <c r="ALL44"/>
     </row>
     <row r="45" spans="1:1000" ht="15">
-      <c r="A45" s="50">
+      <c r="A45" s="42">
         <v>6</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="52" t="s">
+      <c r="C45" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="51"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="43"/>
       <c r="ALE45"/>
       <c r="ALF45"/>
       <c r="ALG45"/>
@@ -2535,18 +2547,18 @@
       <c r="ALL45"/>
     </row>
     <row r="46" spans="1:1000" ht="15">
-      <c r="A46" s="50">
+      <c r="A46" s="42">
         <v>6</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="52" t="s">
+      <c r="C46" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="51"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="43"/>
       <c r="ALE46"/>
       <c r="ALF46"/>
       <c r="ALG46"/>
@@ -2557,18 +2569,18 @@
       <c r="ALL46"/>
     </row>
     <row r="47" spans="1:1000" ht="15">
-      <c r="A47" s="50">
+      <c r="A47" s="42">
         <v>6</v>
       </c>
-      <c r="B47" s="50" t="s">
+      <c r="B47" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="52" t="s">
+      <c r="C47" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="51"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="43"/>
       <c r="ALE47"/>
       <c r="ALF47"/>
       <c r="ALG47"/>
@@ -2579,18 +2591,18 @@
       <c r="ALL47"/>
     </row>
     <row r="48" spans="1:1000" ht="15">
-      <c r="A48" s="50">
+      <c r="A48" s="42">
         <v>6</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="52" t="s">
+      <c r="C48" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="51"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="43"/>
       <c r="ALE48"/>
       <c r="ALF48"/>
       <c r="ALG48"/>
@@ -2601,18 +2613,18 @@
       <c r="ALL48"/>
     </row>
     <row r="49" spans="1:1000" ht="15">
-      <c r="A49" s="50">
+      <c r="A49" s="42">
         <v>6</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="52" t="s">
+      <c r="C49" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="51"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="43"/>
       <c r="ALE49"/>
       <c r="ALF49"/>
       <c r="ALG49"/>
@@ -2623,18 +2635,18 @@
       <c r="ALL49"/>
     </row>
     <row r="50" spans="1:1000" ht="15">
-      <c r="A50" s="50">
+      <c r="A50" s="42">
         <v>7</v>
       </c>
-      <c r="B50" s="50" t="s">
+      <c r="B50" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="52" t="s">
+      <c r="C50" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="51"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="43"/>
       <c r="ALE50"/>
       <c r="ALF50"/>
       <c r="ALG50"/>
@@ -2645,18 +2657,18 @@
       <c r="ALL50"/>
     </row>
     <row r="51" spans="1:1000" ht="15">
-      <c r="A51" s="50">
+      <c r="A51" s="42">
         <v>7</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="52" t="s">
+      <c r="C51" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="51"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="43"/>
       <c r="ALE51"/>
       <c r="ALF51"/>
       <c r="ALG51"/>
@@ -2667,18 +2679,18 @@
       <c r="ALL51"/>
     </row>
     <row r="52" spans="1:1000" ht="15">
-      <c r="A52" s="50">
+      <c r="A52" s="42">
         <v>7</v>
       </c>
-      <c r="B52" s="50" t="s">
+      <c r="B52" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="52" t="s">
+      <c r="C52" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="51"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="43"/>
       <c r="ALE52"/>
       <c r="ALF52"/>
       <c r="ALG52"/>
@@ -2689,18 +2701,18 @@
       <c r="ALL52"/>
     </row>
     <row r="53" spans="1:1000" ht="15">
-      <c r="A53" s="50">
+      <c r="A53" s="42">
         <v>7</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="52" t="s">
+      <c r="C53" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="D53" s="50"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="51"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="43"/>
       <c r="ALE53"/>
       <c r="ALF53"/>
       <c r="ALG53"/>
@@ -2711,18 +2723,18 @@
       <c r="ALL53"/>
     </row>
     <row r="54" spans="1:1000" ht="15">
-      <c r="A54" s="50">
+      <c r="A54" s="42">
         <v>7</v>
       </c>
-      <c r="B54" s="50" t="s">
+      <c r="B54" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="52" t="s">
+      <c r="C54" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="D54" s="50"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="51"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="43"/>
       <c r="ALE54"/>
       <c r="ALF54"/>
       <c r="ALG54"/>
@@ -2733,18 +2745,18 @@
       <c r="ALL54"/>
     </row>
     <row r="55" spans="1:1000" ht="15">
-      <c r="A55" s="50">
+      <c r="A55" s="42">
         <v>7</v>
       </c>
-      <c r="B55" s="50" t="s">
+      <c r="B55" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="52" t="s">
+      <c r="C55" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="51"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="43"/>
       <c r="ALE55"/>
       <c r="ALF55"/>
       <c r="ALG55"/>
@@ -2755,18 +2767,18 @@
       <c r="ALL55"/>
     </row>
     <row r="56" spans="1:1000" ht="15">
-      <c r="A56" s="50">
+      <c r="A56" s="42">
         <v>7</v>
       </c>
-      <c r="B56" s="50" t="s">
+      <c r="B56" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="52" t="s">
+      <c r="C56" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="51"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="42"/>
+      <c r="F56" s="43"/>
       <c r="ALE56"/>
       <c r="ALF56"/>
       <c r="ALG56"/>
@@ -2777,18 +2789,18 @@
       <c r="ALL56"/>
     </row>
     <row r="57" spans="1:1000" ht="15">
-      <c r="A57" s="50">
+      <c r="A57" s="42">
         <v>7</v>
       </c>
-      <c r="B57" s="50" t="s">
+      <c r="B57" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="52" t="s">
+      <c r="C57" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="51"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="43"/>
       <c r="ALE57"/>
       <c r="ALF57"/>
       <c r="ALG57"/>
@@ -2799,564 +2811,564 @@
       <c r="ALL57"/>
     </row>
     <row r="58" spans="1:1000" ht="15">
-      <c r="A58" s="50">
+      <c r="A58" s="42">
         <v>8</v>
       </c>
-      <c r="B58" s="50" t="s">
+      <c r="B58" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="52" t="s">
+      <c r="C58" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D58" s="50"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="51"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="42"/>
+      <c r="F58" s="43"/>
     </row>
     <row r="59" spans="1:1000" ht="15">
-      <c r="A59" s="50">
+      <c r="A59" s="42">
         <v>8</v>
       </c>
-      <c r="B59" s="50" t="s">
+      <c r="B59" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="52" t="s">
+      <c r="C59" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="51"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="43"/>
     </row>
     <row r="60" spans="1:1000" ht="15">
-      <c r="A60" s="50">
+      <c r="A60" s="42">
         <v>8</v>
       </c>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="52" t="s">
+      <c r="C60" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D60" s="50"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="51"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="43"/>
     </row>
     <row r="61" spans="1:1000" ht="15">
-      <c r="A61" s="50">
+      <c r="A61" s="42">
         <v>8</v>
       </c>
-      <c r="B61" s="50" t="s">
+      <c r="B61" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="52" t="s">
+      <c r="C61" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="51"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="43"/>
     </row>
     <row r="62" spans="1:1000" ht="15">
-      <c r="A62" s="50">
+      <c r="A62" s="42">
         <v>8</v>
       </c>
-      <c r="B62" s="50" t="s">
+      <c r="B62" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="52" t="s">
+      <c r="C62" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="D62" s="50"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="51"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="42"/>
+      <c r="F62" s="43"/>
     </row>
     <row r="63" spans="1:1000" ht="15">
-      <c r="A63" s="50">
+      <c r="A63" s="42">
         <v>8</v>
       </c>
-      <c r="B63" s="50" t="s">
+      <c r="B63" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="52" t="s">
+      <c r="C63" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="D63" s="50"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="51"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="43"/>
     </row>
     <row r="64" spans="1:1000" ht="15">
-      <c r="A64" s="50">
+      <c r="A64" s="42">
         <v>8</v>
       </c>
-      <c r="B64" s="50" t="s">
+      <c r="B64" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="52" t="s">
+      <c r="C64" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="D64" s="50"/>
-      <c r="E64" s="50"/>
-      <c r="F64" s="51"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="43"/>
     </row>
     <row r="65" spans="1:6" ht="15">
-      <c r="A65" s="50">
+      <c r="A65" s="42">
         <v>8</v>
       </c>
-      <c r="B65" s="50" t="s">
+      <c r="B65" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="52" t="s">
+      <c r="C65" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="D65" s="50"/>
-      <c r="E65" s="50"/>
-      <c r="F65" s="51"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="43"/>
     </row>
     <row r="66" spans="1:6" ht="15">
-      <c r="A66" s="50">
+      <c r="A66" s="42">
         <v>9</v>
       </c>
-      <c r="B66" s="50" t="s">
+      <c r="B66" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="52" t="s">
+      <c r="C66" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D66" s="50"/>
-      <c r="E66" s="50"/>
-      <c r="F66" s="51"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="43"/>
     </row>
     <row r="67" spans="1:6" ht="15">
-      <c r="A67" s="50">
+      <c r="A67" s="42">
         <v>9</v>
       </c>
-      <c r="B67" s="50" t="s">
+      <c r="B67" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="52" t="s">
+      <c r="C67" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="50"/>
-      <c r="E67" s="50"/>
-      <c r="F67" s="51"/>
+      <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="43"/>
     </row>
     <row r="68" spans="1:6" ht="15">
-      <c r="A68" s="50">
+      <c r="A68" s="42">
         <v>9</v>
       </c>
-      <c r="B68" s="50" t="s">
+      <c r="B68" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C68" s="52" t="s">
+      <c r="C68" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="D68" s="50"/>
-      <c r="E68" s="50"/>
-      <c r="F68" s="51"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="43"/>
     </row>
     <row r="69" spans="1:6" ht="15">
-      <c r="A69" s="50">
+      <c r="A69" s="42">
         <v>9</v>
       </c>
-      <c r="B69" s="50" t="s">
+      <c r="B69" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C69" s="52" t="s">
+      <c r="C69" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="D69" s="50"/>
-      <c r="E69" s="50"/>
-      <c r="F69" s="51"/>
+      <c r="D69" s="42"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="43"/>
     </row>
     <row r="70" spans="1:6" ht="15">
-      <c r="A70" s="50">
+      <c r="A70" s="42">
         <v>9</v>
       </c>
-      <c r="B70" s="50" t="s">
+      <c r="B70" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C70" s="52" t="s">
+      <c r="C70" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="D70" s="50"/>
-      <c r="E70" s="50"/>
-      <c r="F70" s="51"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="43"/>
     </row>
     <row r="71" spans="1:6" ht="15">
-      <c r="A71" s="50">
+      <c r="A71" s="42">
         <v>9</v>
       </c>
-      <c r="B71" s="50" t="s">
+      <c r="B71" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C71" s="52" t="s">
+      <c r="C71" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="D71" s="50"/>
-      <c r="E71" s="50"/>
-      <c r="F71" s="51"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="42"/>
+      <c r="F71" s="43"/>
     </row>
     <row r="72" spans="1:6" ht="15">
-      <c r="A72" s="50">
+      <c r="A72" s="42">
         <v>9</v>
       </c>
-      <c r="B72" s="50" t="s">
+      <c r="B72" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="52" t="s">
+      <c r="C72" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="D72" s="50"/>
-      <c r="E72" s="50"/>
-      <c r="F72" s="51"/>
+      <c r="D72" s="42"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="43"/>
     </row>
     <row r="73" spans="1:6" ht="15">
-      <c r="A73" s="50">
+      <c r="A73" s="42">
         <v>9</v>
       </c>
-      <c r="B73" s="50" t="s">
+      <c r="B73" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="52" t="s">
+      <c r="C73" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="D73" s="50"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="51"/>
+      <c r="D73" s="42"/>
+      <c r="E73" s="42"/>
+      <c r="F73" s="43"/>
     </row>
     <row r="74" spans="1:6" ht="15">
-      <c r="A74" s="50">
+      <c r="A74" s="42">
         <v>10</v>
       </c>
-      <c r="B74" s="50" t="s">
+      <c r="B74" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C74" s="52" t="s">
+      <c r="C74" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="D74" s="50"/>
-      <c r="E74" s="50"/>
-      <c r="F74" s="51"/>
+      <c r="D74" s="42"/>
+      <c r="E74" s="42"/>
+      <c r="F74" s="43"/>
     </row>
     <row r="75" spans="1:6" ht="15">
-      <c r="A75" s="50">
+      <c r="A75" s="42">
         <v>10</v>
       </c>
-      <c r="B75" s="50" t="s">
+      <c r="B75" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C75" s="52" t="s">
+      <c r="C75" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="D75" s="50"/>
-      <c r="E75" s="50"/>
-      <c r="F75" s="51"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="43"/>
     </row>
     <row r="76" spans="1:6" ht="15">
-      <c r="A76" s="50">
+      <c r="A76" s="42">
         <v>10</v>
       </c>
-      <c r="B76" s="50" t="s">
+      <c r="B76" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="52" t="s">
+      <c r="C76" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="D76" s="50"/>
-      <c r="E76" s="50"/>
-      <c r="F76" s="51"/>
+      <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="43"/>
     </row>
     <row r="77" spans="1:6" ht="15">
-      <c r="A77" s="50">
+      <c r="A77" s="42">
         <v>10</v>
       </c>
-      <c r="B77" s="50" t="s">
+      <c r="B77" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="52" t="s">
+      <c r="C77" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D77" s="50"/>
-      <c r="E77" s="50"/>
-      <c r="F77" s="51"/>
+      <c r="D77" s="42"/>
+      <c r="E77" s="42"/>
+      <c r="F77" s="43"/>
     </row>
     <row r="78" spans="1:6" ht="15">
-      <c r="A78" s="50">
+      <c r="A78" s="42">
         <v>10</v>
       </c>
-      <c r="B78" s="50" t="s">
+      <c r="B78" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C78" s="52" t="s">
+      <c r="C78" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="D78" s="50"/>
-      <c r="E78" s="50"/>
-      <c r="F78" s="51"/>
+      <c r="D78" s="42"/>
+      <c r="E78" s="42"/>
+      <c r="F78" s="43"/>
     </row>
     <row r="79" spans="1:6" ht="15">
-      <c r="A79" s="50">
+      <c r="A79" s="42">
         <v>10</v>
       </c>
-      <c r="B79" s="50" t="s">
+      <c r="B79" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C79" s="52" t="s">
+      <c r="C79" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="D79" s="50"/>
-      <c r="E79" s="50"/>
-      <c r="F79" s="51"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
+      <c r="F79" s="43"/>
     </row>
     <row r="80" spans="1:6" ht="15">
-      <c r="A80" s="50">
+      <c r="A80" s="42">
         <v>10</v>
       </c>
-      <c r="B80" s="50" t="s">
+      <c r="B80" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="52" t="s">
+      <c r="C80" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="D80" s="50"/>
-      <c r="E80" s="50"/>
-      <c r="F80" s="51"/>
+      <c r="D80" s="42"/>
+      <c r="E80" s="42"/>
+      <c r="F80" s="43"/>
     </row>
     <row r="81" spans="1:6" ht="15">
-      <c r="A81" s="50">
+      <c r="A81" s="42">
         <v>10</v>
       </c>
-      <c r="B81" s="50" t="s">
+      <c r="B81" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C81" s="52" t="s">
+      <c r="C81" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="D81" s="50"/>
-      <c r="E81" s="50"/>
-      <c r="F81" s="51"/>
+      <c r="D81" s="42"/>
+      <c r="E81" s="42"/>
+      <c r="F81" s="43"/>
     </row>
     <row r="82" spans="1:6" ht="15">
-      <c r="A82" s="50">
+      <c r="A82" s="42">
         <v>11</v>
       </c>
-      <c r="B82" s="50" t="s">
+      <c r="B82" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C82" s="52" t="s">
+      <c r="C82" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D82" s="50"/>
-      <c r="E82" s="50"/>
-      <c r="F82" s="51"/>
+      <c r="D82" s="42"/>
+      <c r="E82" s="42"/>
+      <c r="F82" s="43"/>
     </row>
     <row r="83" spans="1:6" ht="15">
-      <c r="A83" s="50">
+      <c r="A83" s="42">
         <v>11</v>
       </c>
-      <c r="B83" s="50" t="s">
+      <c r="B83" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C83" s="52" t="s">
+      <c r="C83" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="D83" s="50"/>
-      <c r="E83" s="49"/>
-      <c r="F83" s="51"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="41"/>
+      <c r="F83" s="43"/>
     </row>
     <row r="84" spans="1:6" ht="15">
-      <c r="A84" s="50">
+      <c r="A84" s="42">
         <v>11</v>
       </c>
-      <c r="B84" s="50" t="s">
+      <c r="B84" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C84" s="52" t="s">
+      <c r="C84" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="D84" s="50"/>
-      <c r="E84" s="49"/>
-      <c r="F84" s="51"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="41"/>
+      <c r="F84" s="43"/>
     </row>
     <row r="85" spans="1:6" ht="15">
-      <c r="A85" s="50">
+      <c r="A85" s="42">
         <v>11</v>
       </c>
-      <c r="B85" s="50" t="s">
+      <c r="B85" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C85" s="52" t="s">
+      <c r="C85" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="D85" s="50"/>
-      <c r="E85" s="49"/>
-      <c r="F85" s="51"/>
+      <c r="D85" s="42"/>
+      <c r="E85" s="41"/>
+      <c r="F85" s="43"/>
     </row>
     <row r="86" spans="1:6" ht="15">
-      <c r="A86" s="50">
+      <c r="A86" s="42">
         <v>11</v>
       </c>
-      <c r="B86" s="50" t="s">
+      <c r="B86" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C86" s="52" t="s">
+      <c r="C86" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="D86" s="50"/>
-      <c r="E86" s="49"/>
-      <c r="F86" s="51"/>
+      <c r="D86" s="42"/>
+      <c r="E86" s="41"/>
+      <c r="F86" s="43"/>
     </row>
     <row r="87" spans="1:6" ht="15">
-      <c r="A87" s="50">
+      <c r="A87" s="42">
         <v>11</v>
       </c>
-      <c r="B87" s="50" t="s">
+      <c r="B87" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="52" t="s">
+      <c r="C87" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="D87" s="50"/>
-      <c r="E87" s="49"/>
-      <c r="F87" s="51"/>
+      <c r="D87" s="42"/>
+      <c r="E87" s="41"/>
+      <c r="F87" s="43"/>
     </row>
     <row r="88" spans="1:6" ht="15">
-      <c r="A88" s="50">
+      <c r="A88" s="42">
         <v>11</v>
       </c>
-      <c r="B88" s="50" t="s">
+      <c r="B88" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C88" s="52" t="s">
+      <c r="C88" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="D88" s="50"/>
-      <c r="E88" s="49"/>
-      <c r="F88" s="51"/>
+      <c r="D88" s="42"/>
+      <c r="E88" s="41"/>
+      <c r="F88" s="43"/>
     </row>
     <row r="89" spans="1:6" ht="15">
-      <c r="A89" s="50">
+      <c r="A89" s="42">
         <v>11</v>
       </c>
-      <c r="B89" s="50" t="s">
+      <c r="B89" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C89" s="52" t="s">
+      <c r="C89" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="D89" s="50"/>
-      <c r="E89" s="49"/>
-      <c r="F89" s="51"/>
+      <c r="D89" s="42"/>
+      <c r="E89" s="41"/>
+      <c r="F89" s="43"/>
     </row>
     <row r="90" spans="1:6" ht="15">
-      <c r="A90" s="50">
+      <c r="A90" s="42">
         <v>12</v>
       </c>
-      <c r="B90" s="50" t="s">
+      <c r="B90" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C90" s="52" t="s">
+      <c r="C90" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D90" s="50"/>
-      <c r="E90" s="49"/>
-      <c r="F90" s="51"/>
+      <c r="D90" s="42"/>
+      <c r="E90" s="41"/>
+      <c r="F90" s="43"/>
     </row>
     <row r="91" spans="1:6" ht="15">
-      <c r="A91" s="50">
+      <c r="A91" s="42">
         <v>12</v>
       </c>
-      <c r="B91" s="50" t="s">
+      <c r="B91" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C91" s="52" t="s">
+      <c r="C91" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="D91" s="50"/>
-      <c r="E91" s="49"/>
-      <c r="F91" s="51"/>
+      <c r="D91" s="42"/>
+      <c r="E91" s="41"/>
+      <c r="F91" s="43"/>
     </row>
     <row r="92" spans="1:6" ht="15">
-      <c r="A92" s="50">
+      <c r="A92" s="42">
         <v>12</v>
       </c>
-      <c r="B92" s="50" t="s">
+      <c r="B92" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C92" s="52" t="s">
+      <c r="C92" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D92" s="50"/>
-      <c r="E92" s="49"/>
-      <c r="F92" s="51"/>
+      <c r="D92" s="42"/>
+      <c r="E92" s="41"/>
+      <c r="F92" s="43"/>
     </row>
     <row r="93" spans="1:6" ht="15">
-      <c r="A93" s="50">
+      <c r="A93" s="42">
         <v>12</v>
       </c>
-      <c r="B93" s="50" t="s">
+      <c r="B93" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C93" s="52" t="s">
+      <c r="C93" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="D93" s="50"/>
-      <c r="E93" s="49"/>
-      <c r="F93" s="51"/>
+      <c r="D93" s="42"/>
+      <c r="E93" s="41"/>
+      <c r="F93" s="43"/>
     </row>
     <row r="94" spans="1:6" ht="15">
-      <c r="A94" s="50">
+      <c r="A94" s="42">
         <v>12</v>
       </c>
-      <c r="B94" s="50" t="s">
+      <c r="B94" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C94" s="52" t="s">
+      <c r="C94" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D94" s="50"/>
-      <c r="E94" s="49"/>
-      <c r="F94" s="51"/>
+      <c r="D94" s="42"/>
+      <c r="E94" s="41"/>
+      <c r="F94" s="43"/>
     </row>
     <row r="95" spans="1:6" ht="15">
-      <c r="A95" s="50">
+      <c r="A95" s="42">
         <v>12</v>
       </c>
-      <c r="B95" s="50" t="s">
+      <c r="B95" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C95" s="52" t="s">
+      <c r="C95" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="D95" s="50"/>
-      <c r="E95" s="49"/>
-      <c r="F95" s="51"/>
+      <c r="D95" s="42"/>
+      <c r="E95" s="41"/>
+      <c r="F95" s="43"/>
     </row>
     <row r="96" spans="1:6" ht="15">
-      <c r="A96" s="50">
+      <c r="A96" s="42">
         <v>12</v>
       </c>
-      <c r="B96" s="50" t="s">
+      <c r="B96" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C96" s="52" t="s">
+      <c r="C96" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="D96" s="50"/>
-      <c r="E96" s="49"/>
-      <c r="F96" s="51"/>
+      <c r="D96" s="42"/>
+      <c r="E96" s="41"/>
+      <c r="F96" s="43"/>
     </row>
     <row r="97" spans="1:6" ht="15">
-      <c r="A97" s="50">
+      <c r="A97" s="42">
         <v>12</v>
       </c>
-      <c r="B97" s="50" t="s">
+      <c r="B97" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C97" s="52" t="s">
+      <c r="C97" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="D97" s="50"/>
-      <c r="E97" s="49"/>
-      <c r="F97" s="51"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="41"/>
+      <c r="F97" s="43"/>
     </row>
     <row r="98" spans="1:6" ht="15">
       <c r="E98" s="4"/>
@@ -3386,10 +3398,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -3697,6 +3709,23 @@
         <v>11.6</v>
       </c>
       <c r="E18" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" thickBot="1">
+      <c r="A19" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="47">
+        <v>386.65354000000002</v>
+      </c>
+      <c r="C19" s="48">
+        <v>100</v>
+      </c>
+      <c r="D19" s="48">
+        <v>5</v>
+      </c>
+      <c r="E19" s="40">
         <v>0</v>
       </c>
     </row>
@@ -3712,8 +3741,8 @@
   </sheetPr>
   <dimension ref="A1:AMK29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4761,16 +4790,16 @@
       <c r="AMJ1" s="5"/>
     </row>
     <row r="2" spans="1:1024" s="15" customFormat="1" ht="15">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="50">
         <v>242.405</v>
       </c>
-      <c r="C2" s="48">
+      <c r="C2" s="51">
         <v>2</v>
       </c>
-      <c r="D2" s="48">
+      <c r="D2" s="51">
         <v>5</v>
       </c>
       <c r="E2" s="28">
@@ -4795,16 +4824,16 @@
       <c r="V2" s="14"/>
     </row>
     <row r="3" spans="1:1024" ht="15">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="50">
         <v>270.459</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="51">
         <v>30</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="51">
         <v>5</v>
       </c>
       <c r="E3" s="28">
@@ -4829,16 +4858,16 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:1024" ht="15">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4" s="50">
         <v>268.459</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="51">
         <v>3</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="51">
         <v>5</v>
       </c>
       <c r="E4" s="28">
@@ -4863,16 +4892,16 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:1024" ht="15">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="50">
         <v>298.51299999999998</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="51">
         <v>14</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="51">
         <v>5</v>
       </c>
       <c r="E5" s="28">
@@ -4897,16 +4926,16 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:1024" ht="15">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6" s="50">
         <v>296.51299999999998</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="51">
         <v>41</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="51">
         <v>5</v>
       </c>
       <c r="E6" s="28">
@@ -4931,16 +4960,16 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:1024" ht="15">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7" s="50">
         <v>294.51299999999998</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="51">
         <v>7</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="51">
         <v>5</v>
       </c>
       <c r="E7" s="28">
@@ -4965,16 +4994,16 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:1024" ht="16" thickBot="1">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="42">
+      <c r="B8" s="50">
         <v>292.51299999999998</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="51">
         <v>3</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="51">
         <v>5</v>
       </c>
       <c r="E8" s="28">
@@ -4999,16 +5028,16 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:1024" ht="16" thickBot="1">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9" s="47">
         <v>386.65354000000002</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="48">
         <v>100</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="48">
         <v>5</v>
       </c>
       <c r="E9" s="40">

</xml_diff>